<commit_message>
[ADD] Table de type
</commit_message>
<xml_diff>
--- a/TP-Pokemon/csv/kanto.xlsx
+++ b/TP-Pokemon/csv/kanto.xlsx
@@ -20,14 +20,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Bulbizarre</t>
   </si>
   <si>
-    <t xml:space="preserve">1|2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Herbizarre</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t xml:space="preserve">Dracaufeu</t>
   </si>
   <si>
-    <t xml:space="preserve">3|4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Carapuce</t>
   </si>
   <si>
@@ -64,15 +58,9 @@
     <t xml:space="preserve">Papilusion</t>
   </si>
   <si>
-    <t xml:space="preserve">6|4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aspicot</t>
   </si>
   <si>
-    <t xml:space="preserve">6|2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coconfort</t>
   </si>
   <si>
@@ -82,9 +70,6 @@
     <t xml:space="preserve">Roucool</t>
   </si>
   <si>
-    <t xml:space="preserve">0|4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Roucoups</t>
   </si>
   <si>
@@ -124,15 +109,9 @@
     <t xml:space="preserve">Artikodin</t>
   </si>
   <si>
-    <t xml:space="preserve">9|4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Électhor</t>
   </si>
   <si>
-    <t xml:space="preserve">7|4</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sulfura</t>
   </si>
   <si>
@@ -143,9 +122,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dracolosse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10|4</t>
   </si>
   <si>
     <t xml:space="preserve">Mewtwo</t>
@@ -229,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -239,6 +215,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -259,7 +239,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
@@ -270,7 +250,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.61"/>
   </cols>
@@ -285,28 +265,31 @@
       <c r="C1" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F1" s="0" t="n">
+      <c r="D1" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G1" s="0" t="n">
         <v>45</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>49</v>
       </c>
       <c r="H1" s="0" t="n">
         <v>49</v>
       </c>
       <c r="I1" s="0" t="n">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="J1" s="0" t="n">
         <v>65</v>
       </c>
       <c r="K1" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="L1" s="0" t="n">
         <v>45</v>
       </c>
     </row>
@@ -315,33 +298,36 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="I2" s="0" t="n">
         <v>63</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>80</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>80</v>
       </c>
       <c r="K2" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>60</v>
       </c>
     </row>
@@ -350,33 +336,36 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
+      <c r="D3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>82</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="J3" s="0" t="n">
         <v>100</v>
       </c>
       <c r="K3" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>80</v>
       </c>
     </row>
@@ -385,33 +374,34 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="n">
+      <c r="E4" s="0"/>
+      <c r="F4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="I4" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="L4" s="0" t="n">
         <v>65</v>
       </c>
     </row>
@@ -420,33 +410,34 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="0" t="n">
+      <c r="E5" s="0"/>
+      <c r="F5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="I5" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="J5" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="K5" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="L5" s="0" t="n">
         <v>80</v>
       </c>
     </row>
@@ -455,33 +446,36 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F6" s="0" t="n">
+      <c r="D6" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="I6" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>109</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="K6" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="L6" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -490,33 +484,34 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="n">
+      <c r="E7" s="0"/>
+      <c r="F7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="I7" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="L7" s="0" t="n">
         <v>43</v>
       </c>
     </row>
@@ -525,33 +520,34 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="0" t="n">
+      <c r="E8" s="0"/>
+      <c r="F8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="K8" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="L8" s="0" t="n">
         <v>58</v>
       </c>
     </row>
@@ -560,33 +556,34 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="E9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F9" s="0" t="n">
+      <c r="E9" s="0"/>
+      <c r="F9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="I9" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J9" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="K9" s="0" t="n">
         <v>105</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="L9" s="0" t="n">
         <v>78</v>
       </c>
     </row>
@@ -595,33 +592,34 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="0" t="n">
+      <c r="E10" s="0"/>
+      <c r="F10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="I10" s="0" t="n">
         <v>35</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>20</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>20</v>
       </c>
       <c r="K10" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L10" s="0" t="n">
         <v>45</v>
       </c>
     </row>
@@ -630,33 +628,34 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="D11" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="0" t="n">
+      <c r="E11" s="0"/>
+      <c r="F11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="H11" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="I11" s="0" t="n">
         <v>55</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>25</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>25</v>
       </c>
       <c r="K11" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="L11" s="0" t="n">
         <v>30</v>
       </c>
     </row>
@@ -665,33 +664,36 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="0" t="n">
+      <c r="D12" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="H12" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="I12" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="J12" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="K12" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="K12" s="0" t="n">
+      <c r="L12" s="0" t="n">
         <v>70</v>
       </c>
     </row>
@@ -700,33 +702,36 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="0" t="n">
+      <c r="D13" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="I13" s="0" t="n">
         <v>30</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>20</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>20</v>
       </c>
       <c r="K13" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="L13" s="0" t="n">
         <v>50</v>
       </c>
     </row>
@@ -735,33 +740,36 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="0" t="n">
+      <c r="D14" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="H14" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="I14" s="0" t="n">
         <v>50</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>25</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>25</v>
       </c>
       <c r="K14" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="L14" s="0" t="n">
         <v>35</v>
       </c>
     </row>
@@ -770,33 +778,36 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="0" t="n">
+      <c r="D15" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="H15" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="I15" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="J15" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="K15" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="L15" s="0" t="n">
         <v>75</v>
       </c>
     </row>
@@ -805,33 +816,36 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F16" s="0" t="n">
+      <c r="D16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="H16" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="I16" s="0" t="n">
         <v>40</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>35</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>35</v>
       </c>
       <c r="K16" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="L16" s="0" t="n">
         <v>56</v>
       </c>
     </row>
@@ -840,33 +854,36 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="0" t="n">
+      <c r="D17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="H17" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="I17" s="0" t="n">
         <v>55</v>
-      </c>
-      <c r="I17" s="0" t="n">
-        <v>50</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>50</v>
       </c>
       <c r="K17" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L17" s="0" t="n">
         <v>71</v>
       </c>
     </row>
@@ -875,33 +892,36 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="0" t="n">
+      <c r="D18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="H18" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="I18" s="0" t="n">
         <v>75</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>70</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>70</v>
       </c>
       <c r="K18" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L18" s="0" t="n">
         <v>91</v>
       </c>
     </row>
@@ -910,33 +930,34 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F19" s="0" t="n">
+      <c r="D19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0"/>
+      <c r="F19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="H19" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="I19" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="I19" s="0" t="n">
+      <c r="J19" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="K19" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="K19" s="0" t="n">
+      <c r="L19" s="0" t="n">
         <v>72</v>
       </c>
     </row>
@@ -945,33 +966,34 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="0" t="n">
+      <c r="D20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="0"/>
+      <c r="F20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="H20" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="I20" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="I20" s="0" t="n">
+      <c r="J20" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="K20" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="K20" s="0" t="n">
+      <c r="L20" s="0" t="n">
         <v>97</v>
       </c>
     </row>
@@ -980,33 +1002,36 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F21" s="0" t="n">
+      <c r="D21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="H21" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="I21" s="0" t="n">
         <v>30</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>31</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>31</v>
       </c>
       <c r="K21" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="L21" s="0" t="n">
         <v>70</v>
       </c>
     </row>
@@ -1015,33 +1040,36 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" s="0" t="n">
+      <c r="D22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="H22" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="I22" s="0" t="n">
         <v>65</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>61</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>61</v>
       </c>
       <c r="K22" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="L22" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1050,33 +1078,34 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="D23" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E23" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="0" t="n">
+      <c r="E23" s="0"/>
+      <c r="F23" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="H23" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="I23" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="I23" s="0" t="n">
+      <c r="J23" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="K23" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="K23" s="0" t="n">
+      <c r="L23" s="0" t="n">
         <v>55</v>
       </c>
     </row>
@@ -1085,33 +1114,34 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="D24" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="E24" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" s="0" t="n">
+      <c r="E24" s="0"/>
+      <c r="F24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="H24" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="I24" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="I24" s="0" t="n">
+      <c r="J24" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="K24" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="K24" s="0" t="n">
+      <c r="L24" s="0" t="n">
         <v>80</v>
       </c>
     </row>
@@ -1120,33 +1150,34 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="D25" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" s="0" t="n">
+      <c r="E25" s="0"/>
+      <c r="F25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="H25" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="I25" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="I25" s="0" t="n">
+      <c r="J25" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="K25" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="K25" s="0" t="n">
+      <c r="L25" s="0" t="n">
         <v>120</v>
       </c>
     </row>
@@ -1155,33 +1186,34 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C26" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="D26" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="E26" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" s="0" t="n">
+      <c r="E26" s="0"/>
+      <c r="F26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="H26" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="I26" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="I26" s="0" t="n">
+      <c r="J26" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="K26" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="K26" s="0" t="n">
+      <c r="L26" s="0" t="n">
         <v>110</v>
       </c>
     </row>
@@ -1190,33 +1222,34 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C27" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="D27" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" s="0" t="n">
+      <c r="E27" s="0"/>
+      <c r="F27" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="H27" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="I27" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="I27" s="0" t="n">
+      <c r="J27" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="J27" s="0" t="n">
+      <c r="K27" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="K27" s="0" t="n">
+      <c r="L27" s="0" t="n">
         <v>40</v>
       </c>
     </row>
@@ -1225,33 +1258,34 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C28" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="D28" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="E28" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F28" s="0" t="n">
+      <c r="E28" s="0"/>
+      <c r="F28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="G28" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="H28" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="I28" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="I28" s="0" t="n">
+      <c r="J28" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="J28" s="0" t="n">
+      <c r="K28" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="K28" s="0" t="n">
+      <c r="L28" s="0" t="n">
         <v>65</v>
       </c>
     </row>
@@ -1260,33 +1294,36 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E29" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F29" s="0" t="n">
+      <c r="D29" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F29" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="H29" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="H29" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="I29" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="J29" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="J29" s="0" t="n">
+      <c r="K29" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="K29" s="0" t="n">
+      <c r="L29" s="0" t="n">
         <v>85</v>
       </c>
     </row>
@@ -1295,33 +1332,36 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C30" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E30" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F30" s="0" t="n">
-        <v>90</v>
+      <c r="D30" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F30" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G30" s="0" t="n">
         <v>90</v>
       </c>
       <c r="H30" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="I30" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="I30" s="0" t="n">
+      <c r="J30" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="J30" s="0" t="n">
+      <c r="K30" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="K30" s="0" t="n">
+      <c r="L30" s="0" t="n">
         <v>100</v>
       </c>
     </row>
@@ -1330,33 +1370,36 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C31" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="0" t="n">
+      <c r="D31" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F31" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="H31" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="I31" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="I31" s="0" t="n">
+      <c r="J31" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="J31" s="0" t="n">
+      <c r="K31" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="L31" s="0" t="n">
         <v>90</v>
       </c>
     </row>
@@ -1365,33 +1408,34 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C32" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="D32" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="E32" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="0" t="n">
+      <c r="E32" s="0"/>
+      <c r="F32" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="H32" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="I32" s="0" t="n">
         <v>45</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>50</v>
       </c>
       <c r="J32" s="0" t="n">
         <v>50</v>
       </c>
       <c r="K32" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="L32" s="0" t="n">
         <v>50</v>
       </c>
     </row>
@@ -1400,33 +1444,34 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C33" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="D33" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="E33" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F33" s="0" t="n">
+      <c r="E33" s="0"/>
+      <c r="F33" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="H33" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="I33" s="0" t="n">
         <v>65</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>70</v>
       </c>
       <c r="J33" s="0" t="n">
         <v>70</v>
       </c>
       <c r="K33" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="L33" s="0" t="n">
         <v>70</v>
       </c>
     </row>
@@ -1435,33 +1480,36 @@
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C34" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F34" s="0" t="n">
+      <c r="D34" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F34" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="0" t="n">
         <v>91</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="H34" s="0" t="n">
         <v>134</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="I34" s="0" t="n">
         <v>95</v>
       </c>
-      <c r="I34" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="J34" s="0" t="n">
         <v>100</v>
       </c>
       <c r="K34" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L34" s="0" t="n">
         <v>80</v>
       </c>
     </row>
@@ -1470,33 +1518,34 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="D35" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="E35" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="0" t="n">
+      <c r="E35" s="0"/>
+      <c r="F35" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="0" t="n">
         <v>106</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="H35" s="0" t="n">
         <v>110</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="I35" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="I35" s="0" t="n">
+      <c r="J35" s="0" t="n">
         <v>154</v>
       </c>
-      <c r="J35" s="0" t="n">
+      <c r="K35" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="K35" s="0" t="n">
+      <c r="L35" s="0" t="n">
         <v>130</v>
       </c>
     </row>
@@ -1505,19 +1554,17 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="D36" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="E36" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="0" t="n">
-        <v>100</v>
+      <c r="E36" s="0"/>
+      <c r="F36" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="G36" s="0" t="n">
         <v>100</v>
@@ -1532,6 +1579,9 @@
         <v>100</v>
       </c>
       <c r="K36" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="L36" s="0" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[ADD] Dresseur et Arène(Client/Serveur) sans rien implémenté encore
</commit_message>
<xml_diff>
--- a/TP-Pokemon/csv/kanto.xlsx
+++ b/TP-Pokemon/csv/kanto.xlsx
@@ -20,11 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t xml:space="preserve">Bulbizarre</t>
   </si>
   <si>
+    <t xml:space="preserve">PLANT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POISON</t>
+  </si>
+  <si>
     <t xml:space="preserve">Herbizarre</t>
   </si>
   <si>
@@ -34,15 +40,24 @@
     <t xml:space="preserve">Salamèche</t>
   </si>
   <si>
+    <t xml:space="preserve">FIRE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reptincel</t>
   </si>
   <si>
     <t xml:space="preserve">Dracaufeu</t>
   </si>
   <si>
+    <t xml:space="preserve">FLYING</t>
+  </si>
+  <si>
     <t xml:space="preserve">Carapuce</t>
   </si>
   <si>
+    <t xml:space="preserve">WATER</t>
+  </si>
+  <si>
     <t xml:space="preserve">Carabaffe</t>
   </si>
   <si>
@@ -52,6 +67,9 @@
     <t xml:space="preserve">Chenipan</t>
   </si>
   <si>
+    <t xml:space="preserve">BUG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chrysacier</t>
   </si>
   <si>
@@ -70,6 +88,9 @@
     <t xml:space="preserve">Roucool</t>
   </si>
   <si>
+    <t xml:space="preserve">NORMAL</t>
+  </si>
+  <si>
     <t xml:space="preserve">Roucoups</t>
   </si>
   <si>
@@ -97,18 +118,27 @@
     <t xml:space="preserve">Pikachu</t>
   </si>
   <si>
+    <t xml:space="preserve">ELECTRIC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raichu</t>
   </si>
   <si>
     <t xml:space="preserve">Sabelette</t>
   </si>
   <si>
+    <t xml:space="preserve">GROUND</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sablaireau</t>
   </si>
   <si>
     <t xml:space="preserve">Artikodin</t>
   </si>
   <si>
+    <t xml:space="preserve">ICE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Électhor</t>
   </si>
   <si>
@@ -118,6 +148,9 @@
     <t xml:space="preserve">Minidraco</t>
   </si>
   <si>
+    <t xml:space="preserve">DRAGON</t>
+  </si>
+  <si>
     <t xml:space="preserve">Draco</t>
   </si>
   <si>
@@ -125,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mewtwo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSY</t>
   </si>
   <si>
     <t xml:space="preserve">Mew</t>
@@ -134,10 +170,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
+    <numFmt numFmtId="166" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
+    <numFmt numFmtId="167" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -218,7 +255,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -239,10 +276,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D:D"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -250,7 +287,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="10.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="10.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.61"/>
   </cols>
@@ -262,16 +299,18 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E1" s="0" t="n">
+      <c r="C1" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="b">
+      <c r="F1" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G1" s="0" t="n">
@@ -292,24 +331,27 @@
       <c r="L1" s="0" t="n">
         <v>45</v>
       </c>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="b">
+      <c r="F2" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G2" s="0" t="n">
@@ -336,18 +378,20 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="2" t="b">
+      <c r="F3" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G3" s="0" t="n">
@@ -374,16 +418,18 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="0"/>
-      <c r="F4" s="2" t="b">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G4" s="0" t="n">
@@ -410,16 +456,18 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="0"/>
-      <c r="F5" s="2" t="b">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G5" s="0" t="n">
@@ -446,18 +494,20 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" s="2" t="b">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G6" s="0" t="n">
@@ -484,16 +534,18 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E7" s="0"/>
-      <c r="F7" s="2" t="b">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G7" s="0" t="n">
@@ -520,16 +572,18 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E8" s="0"/>
-      <c r="F8" s="2" t="b">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G8" s="0" t="n">
@@ -556,16 +610,18 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>5</v>
-      </c>
-      <c r="E9" s="0"/>
-      <c r="F9" s="2" t="b">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G9" s="0" t="n">
@@ -592,16 +648,18 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" s="0"/>
-      <c r="F10" s="2" t="b">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G10" s="0" t="n">
@@ -628,16 +686,18 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E11" s="0"/>
-      <c r="F11" s="2" t="b">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G11" s="0" t="n">
@@ -664,18 +724,20 @@
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2" t="b">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G12" s="0" t="n">
@@ -702,18 +764,20 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E13" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="2" t="b">
+      <c r="F13" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G13" s="0" t="n">
@@ -740,18 +804,20 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E14" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="2" t="b">
+      <c r="F14" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G14" s="0" t="n">
@@ -778,18 +844,20 @@
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E15" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="2" t="b">
+      <c r="F15" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G15" s="0" t="n">
@@ -816,18 +884,20 @@
         <v>16</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F16" s="2" t="b">
+        <v>21</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G16" s="0" t="n">
@@ -854,18 +924,20 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F17" s="2" t="b">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
@@ -892,18 +964,20 @@
         <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F18" s="2" t="b">
+        <v>24</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G18" s="0" t="n">
@@ -930,16 +1004,18 @@
         <v>19</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" s="0"/>
-      <c r="F19" s="2" t="b">
+        <v>25</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G19" s="0" t="n">
@@ -966,16 +1042,18 @@
         <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" s="0"/>
-      <c r="F20" s="2" t="b">
+        <v>26</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G20" s="0" t="n">
@@ -1002,18 +1080,20 @@
         <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F21" s="2" t="b">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G21" s="0" t="n">
@@ -1040,18 +1120,20 @@
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F22" s="2" t="b">
+        <v>28</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G22" s="0" t="n">
@@ -1078,16 +1160,18 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E23" s="0"/>
-      <c r="F23" s="2" t="b">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G23" s="0" t="n">
@@ -1114,16 +1198,18 @@
         <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E24" s="0"/>
-      <c r="F24" s="2" t="b">
+        <v>30</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G24" s="0" t="n">
@@ -1150,16 +1236,18 @@
         <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="E25" s="0"/>
-      <c r="F25" s="2" t="b">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G25" s="0" t="n">
@@ -1186,16 +1274,18 @@
         <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="E26" s="0"/>
-      <c r="F26" s="2" t="b">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="1"/>
+      <c r="F26" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G26" s="0" t="n">
@@ -1222,16 +1312,18 @@
         <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="E27" s="0"/>
-      <c r="F27" s="2" t="b">
+        <v>34</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G27" s="0" t="n">
@@ -1258,16 +1350,18 @@
         <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="3" t="n">
-        <v>8</v>
-      </c>
-      <c r="E28" s="0"/>
-      <c r="F28" s="2" t="b">
+        <v>36</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G28" s="0" t="n">
@@ -1294,18 +1388,20 @@
         <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F29" s="2" t="b">
+      <c r="F29" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G29" s="0" t="n">
@@ -1332,18 +1428,20 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="3" t="n">
-        <v>7</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F30" s="2" t="b">
+        <v>39</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G30" s="0" t="n">
@@ -1370,18 +1468,20 @@
         <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E31" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F31" s="2" t="b">
+        <v>40</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G31" s="0" t="n">
@@ -1408,16 +1508,18 @@
         <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E32" s="0"/>
-      <c r="F32" s="2" t="b">
+        <v>41</v>
+      </c>
+      <c r="C32" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G32" s="0" t="n">
@@ -1444,16 +1546,18 @@
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E33" s="0"/>
-      <c r="F33" s="2" t="b">
+        <v>43</v>
+      </c>
+      <c r="C33" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G33" s="0" t="n">
@@ -1480,18 +1584,20 @@
         <v>34</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F34" s="2" t="b">
+        <v>44</v>
+      </c>
+      <c r="C34" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="G34" s="0" t="n">
@@ -1518,16 +1624,18 @@
         <v>35</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="E35" s="0"/>
-      <c r="F35" s="2" t="b">
+        <v>45</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G35" s="0" t="n">
@@ -1554,16 +1662,18 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="E36" s="0"/>
-      <c r="F36" s="2" t="b">
+        <v>47</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="3" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="G36" s="0" t="n">

</xml_diff>

<commit_message>
[ADD] Evoluer et attaquer
</commit_message>
<xml_diff>
--- a/TP-Pokemon/csv/kanto.xlsx
+++ b/TP-Pokemon/csv/kanto.xlsx
@@ -160,7 +160,7 @@
     <t xml:space="preserve">Mewtwo</t>
   </si>
   <si>
-    <t xml:space="preserve">PSY</t>
+    <t xml:space="preserve">PSYCHIC</t>
   </si>
   <si>
     <t xml:space="preserve">Mew</t>
@@ -174,7 +174,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
-    <numFmt numFmtId="167" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
+    <numFmt numFmtId="167" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -278,8 +278,8 @@
   </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
[FIX] Récupération de plusieurs joueurs par Save
</commit_message>
<xml_diff>
--- a/TP-Pokemon/csv/kanto.xlsx
+++ b/TP-Pokemon/csv/kanto.xlsx
@@ -170,11 +170,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
-    <numFmt numFmtId="167" formatCode="&quot;BOOL&quot;E&quot;AN&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -242,7 +241,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -252,10 +251,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -278,8 +273,8 @@
   </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -299,7 +294,7 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="n">
+      <c r="C1" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -309,7 +304,7 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="n">
+      <c r="F1" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -331,7 +326,7 @@
       <c r="L1" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="M1" s="3"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -340,7 +335,7 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -350,7 +345,7 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -380,7 +375,7 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -390,7 +385,7 @@
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -420,7 +415,7 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -428,7 +423,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -458,7 +453,7 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -466,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -496,7 +491,7 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -506,7 +501,7 @@
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -536,7 +531,7 @@
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -544,7 +539,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -574,7 +569,7 @@
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -582,7 +577,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -612,7 +607,7 @@
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -620,7 +615,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="1"/>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -650,7 +645,7 @@
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -658,7 +653,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -688,7 +683,7 @@
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -696,7 +691,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="3" t="n">
+      <c r="F11" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -726,7 +721,7 @@
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -736,7 +731,7 @@
       <c r="E12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="3" t="n">
+      <c r="F12" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -766,7 +761,7 @@
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -776,7 +771,7 @@
       <c r="E13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="3" t="n">
+      <c r="F13" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -806,7 +801,7 @@
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -816,7 +811,7 @@
       <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="3" t="n">
+      <c r="F14" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -846,7 +841,7 @@
       <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -856,7 +851,7 @@
       <c r="E15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="3" t="n">
+      <c r="F15" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -886,7 +881,7 @@
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -896,7 +891,7 @@
       <c r="E16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F16" s="3" t="n">
+      <c r="F16" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -926,7 +921,7 @@
       <c r="B17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -936,7 +931,7 @@
       <c r="E17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -966,7 +961,7 @@
       <c r="B18" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -976,7 +971,7 @@
       <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="3" t="n">
+      <c r="F18" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1006,7 +1001,7 @@
       <c r="B19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1014,7 +1009,7 @@
         <v>22</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="3" t="n">
+      <c r="F19" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1044,7 +1039,7 @@
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1052,7 +1047,7 @@
         <v>22</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1082,7 +1077,7 @@
       <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1092,7 +1087,7 @@
       <c r="E21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="3" t="n">
+      <c r="F21" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1122,7 +1117,7 @@
       <c r="B22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1132,7 +1127,7 @@
       <c r="E22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1162,15 +1157,15 @@
       <c r="B23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1200,15 +1195,15 @@
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="3" t="n">
+      <c r="F24" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1238,7 +1233,7 @@
       <c r="B25" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1246,7 +1241,7 @@
         <v>32</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="3" t="n">
+      <c r="F25" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1276,7 +1271,7 @@
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1284,7 +1279,7 @@
         <v>32</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="3" t="n">
+      <c r="F26" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1314,7 +1309,7 @@
       <c r="B27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="3" t="n">
+      <c r="C27" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1322,7 +1317,7 @@
         <v>35</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="3" t="n">
+      <c r="F27" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1352,7 +1347,7 @@
       <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="3" t="n">
+      <c r="C28" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1360,7 +1355,7 @@
         <v>35</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="3" t="n">
+      <c r="F28" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1390,7 +1385,7 @@
       <c r="B29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1400,7 +1395,7 @@
       <c r="E29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="3" t="n">
+      <c r="F29" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1430,7 +1425,7 @@
       <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1440,7 +1435,7 @@
       <c r="E30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="3" t="n">
+      <c r="F30" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1470,7 +1465,7 @@
       <c r="B31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="3" t="n">
+      <c r="C31" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1480,7 +1475,7 @@
       <c r="E31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1510,7 +1505,7 @@
       <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="3" t="n">
+      <c r="C32" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1518,7 +1513,7 @@
         <v>42</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="3" t="n">
+      <c r="F32" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1548,7 +1543,7 @@
       <c r="B33" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1556,7 +1551,7 @@
         <v>42</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="3" t="n">
+      <c r="F33" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1586,7 +1581,7 @@
       <c r="B34" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1596,7 +1591,7 @@
       <c r="E34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="3" t="n">
+      <c r="F34" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1626,7 +1621,7 @@
       <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1634,7 +1629,7 @@
         <v>46</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="3" t="n">
+      <c r="F35" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1664,7 +1659,7 @@
       <c r="B36" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -1672,7 +1667,7 @@
         <v>46</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="3" t="n">
+      <c r="F36" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>